<commit_message>
updates monthly dry outlook table
</commit_message>
<xml_diff>
--- a/metadata/monthly-dry-outlook-metadata.xlsx
+++ b/metadata/monthly-dry-outlook-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/urban-water-drought-data/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCE60A0-AAC6-A040-A0BD-2B03D6008611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F6C55A-FD91-7F48-B6A8-0E891968699F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29040" yWindow="500" windowWidth="27260" windowHeight="27020" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="69120" yWindow="1120" windowWidth="27260" windowHeight="27020" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -85,30 +85,18 @@
     <t>month</t>
   </si>
   <si>
-    <t>acre_feet</t>
-  </si>
-  <si>
     <t>org_id</t>
   </si>
   <si>
     <t>DWR assigned ID number associated with the urban retail water supplier</t>
   </si>
   <si>
-    <t>ID number associated with water system in the supplier service area</t>
-  </si>
-  <si>
     <t>is_annual</t>
   </si>
   <si>
     <t>TRUE if represents an annual value. FALSE for monthly values. Annual values are included in this table and can be quickly identified by filtering the dataset using this field.</t>
   </si>
   <si>
-    <t>The month associated with the shortage action. Annual is included as a month level.</t>
-  </si>
-  <si>
-    <t>shortage_action_type</t>
-  </si>
-  <si>
     <t>nominal</t>
   </si>
   <si>
@@ -121,19 +109,62 @@
     <t>YYYY</t>
   </si>
   <si>
-    <t>The shortage action type. If no action is implemented then "no action". Levels = c("supply augmentation", "demand reduction", "no action")</t>
-  </si>
-  <si>
     <t>ratio</t>
   </si>
   <si>
     <t>numeric</t>
   </si>
   <si>
-    <t>Calendar year associated with the month. AWSDA reports cover July through June. For instance in the 2022 reporting year, this would cover July 2022 through June 2023. Annual values are assigned the year corresponding to the start month; in this case 2022.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The volume of water (acre feet) calculated by subtracting the anticipated unconstrained demand from the anticipated unconstrained supply. When the "shortage_action_type" is "no action" this represents the water surplus or shortage when no action is applied. </t>
+    <t>supplier_name</t>
+  </si>
+  <si>
+    <t>Name of water supplier # TODO is there a more detailed description of this</t>
+  </si>
+  <si>
+    <t>ID number associated with water system in the supplier service area #TODO decide if we want to include this</t>
+  </si>
+  <si>
+    <t>Calendar year associated with the month. AWSDA reports cover July through June. For instance in the 2022 reporting year, this would cover July 2022 through June 2023. Annual values are assigned the year corresponding to the start month; in this case 2022. Levels = c(2022, 2023)</t>
+  </si>
+  <si>
+    <t>The month associated with the shortage action. Annual is included as a month level. Levels = c("jul", "aug", "sep", "oct", "nov", "dec", "jan", "feb", "mar", 
+"apr", "may", "jun", "annual")</t>
+  </si>
+  <si>
+    <t>is_wscp_action</t>
+  </si>
+  <si>
+    <t>TRUE represents shortage (or surplus) values associated with implementing supply or demand actions (Water Shortage Contingency Plan actions). FALSE represents shortage (or surplus) values associated with no WSCP actions.</t>
+  </si>
+  <si>
+    <t>shortage_surplus_acre_feet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The volume of water (acre feet) calculated by subtracting the anticipated unconstrained demand from the anticipated unconstrained supply. This calculated field is part of the AWSDA reporting. </t>
+  </si>
+  <si>
+    <t>shortage_surplus_percent</t>
+  </si>
+  <si>
+    <t>The percentage of water shortage calculated by subtracting the anticipated unconstrained demand from the anticipated unconstrained supply divided by the unconstrained deman and multiplied by 100. This monthly number indicates the percent water supplies are short (or in surplus if positive). This value is used to determine the State Standard Shortage Level.</t>
+  </si>
+  <si>
+    <t>state_standard_shortage_level</t>
+  </si>
+  <si>
+    <t># TODO need a good definition for this</t>
+  </si>
+  <si>
+    <t>benefit_demand_reduction_acre_feet</t>
+  </si>
+  <si>
+    <t>benefit_supply_augmentation_acre_feet</t>
+  </si>
+  <si>
+    <t>Additional water quanity (acre feet) resulting from a supply augmentation action. This will be NA when is_wscp_action is FALSE</t>
+  </si>
+  <si>
+    <t>Additional water quanity (acre feet) resulting from a demand reduction action. This will be NA when is_wscp_action is FALSE</t>
   </si>
 </sst>
 </file>
@@ -182,20 +213,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AMG11"/>
+  <dimension ref="A1:AMG13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -589,15 +616,15 @@
     <col min="1" max="1" width="19.6640625" style="1"/>
     <col min="2" max="2" width="65" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="16" style="3" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" style="3" customWidth="1"/>
-    <col min="12" max="13" width="9.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" style="1" customWidth="1"/>
+    <col min="12" max="13" width="9.1640625" style="1" customWidth="1"/>
     <col min="14" max="1021" width="19.6640625" style="1"/>
     <col min="1022" max="1024" width="8.33203125" customWidth="1"/>
   </cols>
@@ -612,171 +639,244 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="5"/>
-    </row>
-    <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="1">
+        <v>2022</v>
+      </c>
+      <c r="M5" s="1">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="3">
-        <v>2022</v>
-      </c>
-      <c r="M4" s="3">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="3">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="1">
         <v>-812606</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M9" s="1">
         <v>3419874</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G11" s="6"/>
+    <row r="10" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="1">
+        <v>-99.889520000000005</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1022" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C10 C14:C1024" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1022" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E10 E14:E1024" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1022" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1024" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>